<commit_message>
nb_plot_hodl as the main analysis tool
</commit_message>
<xml_diff>
--- a/output/binance_BTCUSDT_results_raw.xlsx
+++ b/output/binance_BTCUSDT_results_raw.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800"/>
+    <workbookView windowWidth="19200" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="binance_BTCUSDT_results" sheetId="1" r:id="rId1"/>
@@ -9594,7 +9594,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -9766,12 +9766,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10037,16 +10031,16 @@
     <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -10607,8 +10601,8 @@
   <sheetPr/>
   <dimension ref="A1:V636"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="A451" workbookViewId="0">
-      <selection activeCell="K460" sqref="K460"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="A234" workbookViewId="0">
+      <selection activeCell="J638" sqref="J638"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14.5"/>

</xml_diff>